<commit_message>
Update ML-DL-LLMs ver 0.2 - session progress.xlsx
</commit_message>
<xml_diff>
--- a/ML-DL-LLMs ver 0.2 - session progress.xlsx
+++ b/ML-DL-LLMs ver 0.2 - session progress.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gridflowAI\cgi-AI-ML-GenAI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E3C79A-831A-4688-9D60-F2E54A7534B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C562B1A-8444-413F-B9E1-7B8DF4A7DDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30885" yWindow="-8730" windowWidth="20025" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30885" yWindow="-7200" windowWidth="16095" windowHeight="12435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="261">
   <si>
     <t>AI Fundamentatals</t>
   </si>
@@ -1141,6 +1141,21 @@
   </si>
   <si>
     <t>09 and 10th</t>
+  </si>
+  <si>
+    <t>EDA</t>
+  </si>
+  <si>
+    <t>Choice of ML</t>
+  </si>
+  <si>
+    <t>CV/ Tuning</t>
+  </si>
+  <si>
+    <t>2. Merc dataset - regression</t>
+  </si>
+  <si>
+    <t>1. CA housing - regression (Group 2)</t>
   </si>
 </sst>
 </file>
@@ -1600,7 +1615,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1767,6 +1782,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1775,12 +1793,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2063,17 +2075,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H188"/>
+  <dimension ref="A1:H195"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A184" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D202" sqref="D202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" style="10" customWidth="1"/>
     <col min="2" max="2" width="25.77734375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" style="10" customWidth="1"/>
+    <col min="3" max="3" width="35.44140625" style="10" customWidth="1"/>
     <col min="4" max="4" width="23.88671875" style="10" customWidth="1"/>
     <col min="5" max="5" width="16.6640625" style="10" customWidth="1"/>
     <col min="6" max="6" width="13" style="44" customWidth="1"/>
@@ -2559,7 +2571,7 @@
       <c r="E34" s="6">
         <v>2</v>
       </c>
-      <c r="F34" s="59" t="s">
+      <c r="F34" s="56" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2632,7 +2644,7 @@
       <c r="E40" s="5">
         <v>0.5</v>
       </c>
-      <c r="F40" s="60">
+      <c r="F40" s="42">
         <v>10</v>
       </c>
     </row>
@@ -3907,7 +3919,7 @@
       <c r="B157" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="C157" s="56" t="s">
+      <c r="C157" s="57" t="s">
         <v>195</v>
       </c>
       <c r="F157" s="42"/>
@@ -3917,7 +3929,7 @@
       <c r="B158" s="32" t="s">
         <v>190</v>
       </c>
-      <c r="C158" s="57"/>
+      <c r="C158" s="58"/>
       <c r="F158" s="42"/>
     </row>
     <row r="159" spans="1:7" ht="72" x14ac:dyDescent="0.3">
@@ -3927,7 +3939,7 @@
       <c r="B159" s="32" t="s">
         <v>191</v>
       </c>
-      <c r="C159" s="57"/>
+      <c r="C159" s="58"/>
       <c r="F159" s="42"/>
     </row>
     <row r="160" spans="1:7" ht="18" x14ac:dyDescent="0.3">
@@ -3935,7 +3947,7 @@
       <c r="B160" s="32" t="s">
         <v>192</v>
       </c>
-      <c r="C160" s="57"/>
+      <c r="C160" s="58"/>
       <c r="F160" s="42"/>
     </row>
     <row r="161" spans="1:6" ht="18" x14ac:dyDescent="0.3">
@@ -3943,7 +3955,7 @@
       <c r="B161" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="C161" s="57"/>
+      <c r="C161" s="58"/>
       <c r="F161" s="42"/>
     </row>
     <row r="162" spans="1:6" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -3951,7 +3963,7 @@
       <c r="B162" s="33" t="s">
         <v>194</v>
       </c>
-      <c r="C162" s="58"/>
+      <c r="C162" s="59"/>
       <c r="F162" s="42"/>
     </row>
     <row r="163" spans="1:6" ht="18" x14ac:dyDescent="0.3">
@@ -3961,7 +3973,7 @@
       <c r="B163" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="C163" s="56" t="s">
+      <c r="C163" s="57" t="s">
         <v>195</v>
       </c>
       <c r="F163" s="42"/>
@@ -3971,7 +3983,7 @@
       <c r="B164" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="C164" s="57"/>
+      <c r="C164" s="58"/>
       <c r="F164" s="42"/>
     </row>
     <row r="165" spans="1:6" ht="54.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -3981,7 +3993,7 @@
       <c r="B165" s="33" t="s">
         <v>200</v>
       </c>
-      <c r="C165" s="58"/>
+      <c r="C165" s="59"/>
       <c r="F165" s="42"/>
     </row>
     <row r="166" spans="1:6" ht="18" x14ac:dyDescent="0.3">
@@ -3991,7 +4003,7 @@
       <c r="B166" s="32" t="s">
         <v>203</v>
       </c>
-      <c r="C166" s="56" t="s">
+      <c r="C166" s="57" t="s">
         <v>195</v>
       </c>
       <c r="F166" s="42"/>
@@ -4001,7 +4013,7 @@
       <c r="B167" s="32" t="s">
         <v>204</v>
       </c>
-      <c r="C167" s="57"/>
+      <c r="C167" s="58"/>
       <c r="F167" s="42"/>
     </row>
     <row r="168" spans="1:6" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -4011,7 +4023,7 @@
       <c r="B168" s="33" t="s">
         <v>205</v>
       </c>
-      <c r="C168" s="58"/>
+      <c r="C168" s="59"/>
       <c r="F168" s="42"/>
     </row>
     <row r="169" spans="1:6" ht="18" x14ac:dyDescent="0.3">
@@ -4021,7 +4033,7 @@
       <c r="B169" s="32" t="s">
         <v>208</v>
       </c>
-      <c r="C169" s="56" t="s">
+      <c r="C169" s="57" t="s">
         <v>211</v>
       </c>
       <c r="F169" s="42"/>
@@ -4031,7 +4043,7 @@
       <c r="B170" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="C170" s="57"/>
+      <c r="C170" s="58"/>
       <c r="F170" s="42"/>
     </row>
     <row r="171" spans="1:6" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
@@ -4041,7 +4053,7 @@
       <c r="B171" s="33" t="s">
         <v>210</v>
       </c>
-      <c r="C171" s="58"/>
+      <c r="C171" s="59"/>
       <c r="F171" s="42"/>
     </row>
     <row r="172" spans="1:6" ht="18" x14ac:dyDescent="0.3">
@@ -4197,6 +4209,40 @@
       <c r="D188" s="54"/>
       <c r="E188" s="55" t="s">
         <v>249</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B191" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C191" s="10" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B192" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="C192" s="10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="193" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B193" s="10" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="194" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B194" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="C194" s="10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B195" s="10" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>